<commit_message>
Combine- has not yet finished
</commit_message>
<xml_diff>
--- a/design-document/AKD-MessageOutput-.xlsx
+++ b/design-document/AKD-MessageOutput-.xlsx
@@ -166,15 +166,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Error</t>
-  </si>
-  <si>
-    <t>That character cannnot used for email address. Please use character (A-Z a-z @._-)</t>
-  </si>
-  <si>
-    <t>{ 0 } is not input</t>
   </si>
   <si>
     <t>Message</t>
@@ -223,24 +217,12 @@
     <t>Thời điểm cấp  {0}  phải trước thời điểm cấp  {1}</t>
   </si>
   <si>
-    <t>{0}  invalid</t>
-  </si>
-  <si>
     <t>Đăng ký tối thiểu 1 buổi học trong tuần</t>
   </si>
   <si>
-    <t>{0} must be not less than 0</t>
-  </si>
-  <si>
-    <t>Export Fail. Error !</t>
-  </si>
-  <si>
     <t xml:space="preserve">{0} phải nhỏ hơn ngày hiện tại </t>
   </si>
   <si>
-    <t>{ 0 } phải lớn hơn hoặc bằng ngày hiện tại</t>
-  </si>
-  <si>
     <t>{ 0 } lỗi xuất file</t>
   </si>
   <si>
@@ -251,6 +233,57 @@
   </si>
   <si>
     <t>AKD-MS0011-E</t>
+  </si>
+  <si>
+    <t>{0} phải lớn hơn 0</t>
+  </si>
+  <si>
+    <t>{ 0 } chưa được nhập</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{0}  không hợp lệ </t>
+  </si>
+  <si>
+    <t>Xuất thư mục bị lỗi</t>
+  </si>
+  <si>
+    <t>{0} nhỏ hơn 20 ký tự</t>
+  </si>
+  <si>
+    <t>AKD-MS0012-E</t>
+  </si>
+  <si>
+    <t>{0} quá dài</t>
+  </si>
+  <si>
+    <t>AKD-MS0013-E</t>
+  </si>
+  <si>
+    <t>AKD-MS0014-E</t>
+  </si>
+  <si>
+    <t>Lưu không thành công</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Giờ Bắt Đầu Dạng HH:MM</t>
+  </si>
+  <si>
+    <t>AKD-MS0015-E</t>
+  </si>
+  <si>
+    <t>{0} Dạng HH:MM</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Không có nội dung để xuất file</t>
+  </si>
+  <si>
+    <t>AKD-MS0016-E</t>
+  </si>
+  <si>
+    <t>{ 0 } phải nhỏ hơn hoặc bằng ngày hiện tại</t>
   </si>
 </sst>
 </file>
@@ -391,7 +424,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
@@ -446,6 +479,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1119,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD14"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="11.35"/>
@@ -1138,23 +1174,23 @@
     <row r="2" spans="1:5" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" s="5"/>
     </row>
@@ -1163,13 +1199,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="13"/>
     </row>
@@ -1178,13 +1214,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E5" s="13"/>
     </row>
@@ -1193,13 +1229,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E6" s="13"/>
     </row>
@@ -1208,13 +1244,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E7" s="13"/>
     </row>
@@ -1223,13 +1259,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E8" s="13"/>
     </row>
@@ -1238,13 +1274,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E9" s="13"/>
     </row>
@@ -1253,13 +1289,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E10" s="13"/>
     </row>
@@ -1268,13 +1304,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E11" s="13"/>
     </row>
@@ -1283,13 +1319,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E12" s="13"/>
     </row>
@@ -1298,13 +1334,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E13" s="13"/>
     </row>
@@ -1313,56 +1349,98 @@
         <v>11</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="A15" s="6">
+        <v>12</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="A16" s="6">
+        <v>13</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>31</v>
+      </c>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="A17" s="6">
+        <v>14</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>34</v>
+      </c>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="A18" s="6">
+        <v>15</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="A19" s="6">
+        <v>16</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>36</v>
+      </c>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="22.5" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="D20" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="22.5" customHeight="1">

</xml_diff>